<commit_message>
Towards debugging new class hierarchy.
</commit_message>
<xml_diff>
--- a/mysite/scisheets/core/test_dir/excel_write.xlsx
+++ b/mysite/scisheets/core/test_dir/excel_write.xlsx
@@ -11,112 +11,6 @@
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>DUMMY1_COLUMN</t>
-  </si>
-  <si>
-    <t>DUMMY2_COLUMN</t>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>three</t>
-  </si>
-</sst>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,55 +294,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="n">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
All tests pass but some problems with single_gene.
</commit_message>
<xml_diff>
--- a/mysite/scisheets/core/test_dir/excel_write.xlsx
+++ b/mysite/scisheets/core/test_dir/excel_write.xlsx
@@ -11,6 +11,129 @@
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>DUMMY1_COLUMN</t>
+  </si>
+  <si>
+    <t>DUMMY2_COLUMN</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt formatCode="General" numFmtId="164"/>
+  </numFmts>
+  <fonts count="6">
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="3" name="Comma" xfId="4"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -294,4 +417,55 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changing relative paths to absolute paths
</commit_message>
<xml_diff>
--- a/mysite/scisheets/core/test_dir/excel_write.xlsx
+++ b/mysite/scisheets/core/test_dir/excel_write.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38,7 +38,7 @@
   <numFmts count="1">
     <numFmt formatCode="General" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -78,6 +78,9 @@
       <b val="1"/>
       <color rgb="00000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,21 +108,24 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+  <cellXfs count="4">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -131,7 +137,6 @@
     <cellStyle builtinId="3" name="Comma" xfId="4"/>
     <cellStyle builtinId="6" name="Comma [0]" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -431,13 +436,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>